<commit_message>
new results for puzzle3
</commit_message>
<xml_diff>
--- a/puzzle3 results.xlsx
+++ b/puzzle3 results.xlsx
@@ -12,19 +12,20 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14235"/>
   </bookViews>
   <sheets>
-    <sheet name="puzzle3 average" sheetId="9" r:id="rId1"/>
-    <sheet name="puzzle3 run1 (5)" sheetId="8" r:id="rId2"/>
-    <sheet name="puzzle3 run1 (4)" sheetId="7" r:id="rId3"/>
-    <sheet name="puzzle3 run1 (3)" sheetId="6" r:id="rId4"/>
-    <sheet name="puzzle3 run1 (2)" sheetId="5" r:id="rId5"/>
-    <sheet name="puzzle3 run1" sheetId="1" r:id="rId6"/>
+    <sheet name="puzzle3 without elitism run1" sheetId="11" r:id="rId1"/>
+    <sheet name="puzzle3 average" sheetId="9" r:id="rId2"/>
+    <sheet name="puzzle3 run1 (5)" sheetId="8" r:id="rId3"/>
+    <sheet name="puzzle3 run1 (4)" sheetId="7" r:id="rId4"/>
+    <sheet name="puzzle3 run1 (3)" sheetId="6" r:id="rId5"/>
+    <sheet name="puzzle3 run1 (2)" sheetId="5" r:id="rId6"/>
+    <sheet name="puzzle3 run1" sheetId="1" r:id="rId7"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="13">
   <si>
     <t xml:space="preserve">     Current Generation</t>
   </si>
@@ -5367,11 +5368,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1838291888"/>
-        <c:axId val="-1838301136"/>
+        <c:axId val="-1140459440"/>
+        <c:axId val="-1140470864"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1838291888"/>
+        <c:axId val="-1140459440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5470,7 +5471,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838301136"/>
+        <c:crossAx val="-1140470864"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5478,7 +5479,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1838301136"/>
+        <c:axId val="-1140470864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5585,7 +5586,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838291888"/>
+        <c:crossAx val="-1140459440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -10427,11 +10428,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="-1838303856"/>
-        <c:axId val="-1838301680"/>
+        <c:axId val="-1140470320"/>
+        <c:axId val="-1141870768"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1838303856"/>
+        <c:axId val="-1140470320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10530,7 +10531,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838301680"/>
+        <c:crossAx val="-1141870768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -10538,7 +10539,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1838301680"/>
+        <c:axId val="-1141870768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -10645,7 +10646,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1838303856"/>
+        <c:crossAx val="-1140470320"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -12166,9 +12167,143 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B19"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>1000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>3000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>4000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>5000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>6000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>7000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>8000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>9000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>11000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>12000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>13000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>14000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>16000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>17000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M270"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
@@ -23591,7 +23726,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M253"/>
   <sheetViews>
@@ -31783,7 +31918,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M253"/>
   <sheetViews>
@@ -39975,7 +40110,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M253"/>
   <sheetViews>
@@ -48167,7 +48302,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M253"/>
   <sheetViews>
@@ -56359,12 +56494,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M243"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>